<commit_message>
Working on the hard problem
</commit_message>
<xml_diff>
--- a/2025 Excel Esports Chille - The Docks of Valparaiso (Juan Jose Cifuentes) - Case and Answers.xlsx
+++ b/2025 Excel Esports Chille - The Docks of Valparaiso (Juan Jose Cifuentes) - Case and Answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29413"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EA05A7-CC62-4AE0-A31D-B35DF57B313F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A512AB-2A44-4366-8A42-908FA8AAC5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{BE4A18CD-9E80-4D14-A39F-1C9BD96D766A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE4A18CD-9E80-4D14-A39F-1C9BD96D766A}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="233">
   <si>
     <t>Juan José Cifuentes</t>
   </si>
@@ -772,6 +772,15 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Unit Value</t>
+  </si>
+  <si>
+    <t>Ship Cargo Type</t>
+  </si>
+  <si>
+    <t>Cargo 1</t>
   </si>
 </sst>
 </file>
@@ -938,7 +947,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -991,8 +1000,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1253,13 +1274,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1438,6 +1485,30 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1523,9 +1594,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="27" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2267,7 +2335,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>916305</xdr:colOff>
+      <xdr:colOff>512445</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>259080</xdr:rowOff>
     </xdr:to>
@@ -2858,8 +2926,8 @@
   <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:AA289"/>
   <sheetViews>
-    <sheetView topLeftCell="A228" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E217" sqref="E217:E236"/>
+    <sheetView tabSelected="1" topLeftCell="P266" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S272" sqref="S272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -2875,44 +2943,46 @@
     <col min="15" max="15" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="15.8984375" style="1"/>
+    <col min="18" max="24" width="15.8984375" style="1"/>
+    <col min="25" max="25" width="16.8984375" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="15.8984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1"/>
     <row r="2" spans="2:13" ht="59.25" customHeight="1">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="75"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1"/>
     <row r="4" spans="2:13" ht="33" customHeight="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="70"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="2:13" ht="196.2" customHeight="1">
       <c r="C5"/>
@@ -2923,10 +2993,10 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:13" ht="33" customHeight="1">
-      <c r="L6" s="68" t="s">
+      <c r="L6" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="70"/>
+      <c r="M6" s="78"/>
     </row>
     <row r="7" spans="2:13" ht="113.4" customHeight="1">
       <c r="K7" s="4"/>
@@ -2934,52 +3004,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
     </row>
     <row r="9" spans="2:13" ht="79.2" customHeight="1">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="2:13" ht="194.4" customHeight="1">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1">
       <c r="B11" s="5"/>
@@ -2996,20 +3066,20 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="70"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="78"/>
     </row>
     <row r="13" spans="2:13" ht="15" customHeight="1">
       <c r="B13" s="8"/>
@@ -3059,15 +3129,15 @@
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="78" t="s">
+      <c r="G16" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="80"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="88"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="16" t="s">
@@ -3081,15 +3151,15 @@
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="81" t="s">
+      <c r="G17" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="16" t="s">
@@ -3103,15 +3173,15 @@
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="73" t="s">
+      <c r="G18" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="16" t="s">
@@ -3125,15 +3195,15 @@
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="16" t="s">
@@ -3147,15 +3217,15 @@
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="73" t="s">
+      <c r="G20" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="16" t="s">
@@ -3169,34 +3239,34 @@
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="74" t="s">
+      <c r="G21" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="76"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="84"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.4">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="70"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="78"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="24"/>
@@ -8689,7 +8759,7 @@
       <c r="O217" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="P217" s="93" t="str">
+      <c r="P217" s="64" t="str">
         <f>_xlfn.XLOOKUP(P216,_tCList[Cargo],_tCList[Cargo Type])</f>
         <v>Dry Bulk</v>
       </c>
@@ -8755,7 +8825,7 @@
       <c r="O218" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="P218" s="93" cm="1">
+      <c r="P218" s="64" cm="1">
         <f t="array" ref="P218:W218">IF(P217:W217=X217,1,0)</f>
         <v>0</v>
       </c>
@@ -9911,7 +9981,7 @@
       <c r="F256" s="20"/>
       <c r="G256" s="28"/>
     </row>
-    <row r="257" spans="2:16" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="257" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B257" s="32" t="s">
         <v>160</v>
       </c>
@@ -9921,7 +9991,7 @@
       <c r="F257" s="20"/>
       <c r="G257" s="28"/>
     </row>
-    <row r="258" spans="2:16" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="258" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B258" s="32" t="s">
         <v>161</v>
       </c>
@@ -9931,7 +10001,7 @@
       <c r="F258" s="20"/>
       <c r="G258" s="28"/>
     </row>
-    <row r="259" spans="2:16" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="259" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="B259" s="29"/>
       <c r="C259" s="20"/>
       <c r="D259" s="20"/>
@@ -9939,7 +10009,7 @@
       <c r="F259" s="20"/>
       <c r="G259" s="28"/>
     </row>
-    <row r="260" spans="2:16" s="11" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
+    <row r="260" spans="2:27" s="11" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
       <c r="B260" s="13" t="s">
         <v>10</v>
       </c>
@@ -9983,11 +10053,30 @@
       <c r="P260" s="13" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="261" spans="2:16" s="11" customFormat="1" ht="15" customHeight="1">
+      <c r="U260" s="65" t="s">
+        <v>229</v>
+      </c>
+      <c r="V260" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="F261" s="20"/>
-    </row>
-    <row r="262" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U261" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="V261" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="W261" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="X261" s="67" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y261"/>
+    </row>
+    <row r="262" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
       <c r="B262" s="35" t="s">
         <v>164</v>
       </c>
@@ -10031,8 +10120,27 @@
       <c r="P262" s="38" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="263" spans="2:16" s="11" customFormat="1" ht="15" customHeight="1">
+      <c r="U262" s="68" t="str" cm="1">
+        <f t="array" aca="1" ref="U262:V262" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U262)*2-2,$V$260,2),$V$260,)</f>
+        <v>Cellulose</v>
+      </c>
+      <c r="V262" s="66">
+        <f ca="1"/>
+        <v>68400</v>
+      </c>
+      <c r="W262" s="66" t="str">
+        <f ca="1">_xlfn.XLOOKUP(U262,_tCList[Cargo],_tCList[Cargo Type])</f>
+        <v>Dry Bulk</v>
+      </c>
+      <c r="X262" s="66">
+        <f ca="1">_xlfn.XLOOKUP(U262,_tCList[Cargo],_tCList[Value per Unit])</f>
+        <v>500</v>
+      </c>
+      <c r="AA262" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="263" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="E263" s="40"/>
       <c r="F263" s="20"/>
       <c r="G263" s="41"/>
@@ -10045,8 +10153,27 @@
       <c r="N263" s="42"/>
       <c r="O263" s="41"/>
       <c r="P263" s="41"/>
-    </row>
-    <row r="264" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U263" s="68" t="str" cm="1">
+        <f t="array" aca="1" ref="U263:V263" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U263)*2-2,$V$260,2),$V$260,)</f>
+        <v>Sulfuric Acid</v>
+      </c>
+      <c r="V263" s="66">
+        <f ca="1"/>
+        <v>7200</v>
+      </c>
+      <c r="W263" s="66" t="str">
+        <f ca="1">_xlfn.XLOOKUP(U263,_tCList[Cargo],_tCList[Cargo Type])</f>
+        <v>Liquid Bulk</v>
+      </c>
+      <c r="X263" s="66">
+        <f ca="1">_xlfn.XLOOKUP(U263,_tCList[Cargo],_tCList[Value per Unit])</f>
+        <v>150</v>
+      </c>
+      <c r="AA263" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="264" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B264" s="43">
         <v>101</v>
       </c>
@@ -10088,8 +10215,27 @@
       <c r="P264" s="38" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="265" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U264" s="68" t="str" cm="1">
+        <f t="array" aca="1" ref="U264:V264" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U264)*2-2,$V$260,2),$V$260,)</f>
+        <v>Salmon</v>
+      </c>
+      <c r="V264" s="66">
+        <f ca="1"/>
+        <v>5760</v>
+      </c>
+      <c r="W264" s="66" t="str">
+        <f ca="1">_xlfn.XLOOKUP(U264,_tCList[Cargo],_tCList[Cargo Type])</f>
+        <v>Container</v>
+      </c>
+      <c r="X264" s="66">
+        <f ca="1">_xlfn.XLOOKUP(U264,_tCList[Cargo],_tCList[Value per Unit])</f>
+        <v>120000</v>
+      </c>
+      <c r="AA264" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="265" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B265" s="43">
         <v>102</v>
       </c>
@@ -10131,8 +10277,24 @@
       <c r="P265" s="38" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="266" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U265" s="69" t="str" cm="1">
+        <f t="array" aca="1" ref="U265:V265" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U265)*2-2,$V$260,2),$V$260,)</f>
+        <v>Iron Ore</v>
+      </c>
+      <c r="V265" s="70">
+        <f ca="1"/>
+        <v>82800</v>
+      </c>
+      <c r="W265" s="70" t="str">
+        <f ca="1">_xlfn.XLOOKUP(U265,_tCList[Cargo],_tCList[Cargo Type])</f>
+        <v>Dry Bulk</v>
+      </c>
+      <c r="X265" s="70">
+        <f ca="1">_xlfn.XLOOKUP(U265,_tCList[Cargo],_tCList[Value per Unit])</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="266" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B266" s="43">
         <v>103</v>
       </c>
@@ -10175,7 +10337,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="267" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="267" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
       <c r="B267" s="43">
         <v>104</v>
       </c>
@@ -10217,8 +10379,21 @@
       <c r="P267" s="38" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="268" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U267" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="V267" s="67" t="s">
+        <v>231</v>
+      </c>
+      <c r="W267" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="X267" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z267"/>
+    </row>
+    <row r="268" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
       <c r="B268" s="43">
         <v>105</v>
       </c>
@@ -10260,8 +10435,36 @@
       <c r="P268" s="38" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="269" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U268" s="66" t="str" cm="1">
+        <f t="array" ref="U268:U279">_xlfn.TEXTSPLIT(INDEX($P$262:$P$283,V260),,";")</f>
+        <v>DBS3</v>
+      </c>
+      <c r="V268" s="66" t="str" cm="1">
+        <f t="array" ref="V268:V279">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(U268),_tCapacity[Model ID],_tCapacity[Cargo Type])</f>
+        <v>Dry Bulk</v>
+      </c>
+      <c r="W268" s="66" cm="1">
+        <f t="array" ref="W268:W279">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(U268),_tCapacity[Model ID],_tCapacity[Capacity])</f>
+        <v>35000</v>
+      </c>
+      <c r="X268" s="11" t="str" cm="1">
+        <f t="array" aca="1" ref="X268:Y271" ca="1">_xlfn._xlws.FILTER(_xlfn.HSTACK(_xlfn.ANCHORARRAY(U268),_xlfn.ANCHORARRAY(W268)),_xlfn.ANCHORARRAY(V268)=W264)</f>
+        <v>CTS2</v>
+      </c>
+      <c r="Y268" s="11">
+        <f ca="1"/>
+        <v>2000</v>
+      </c>
+      <c r="Z268" s="11">
+        <f ca="1">SUM($Y$268:Y268)</f>
+        <v>2000</v>
+      </c>
+      <c r="AA268" s="11" t="str" cm="1">
+        <f t="array" aca="1" ref="AA268" ca="1">INDEX(_xlfn.ANCHORARRAY(X268),_xlfn.XMATCH(V264,$Z$268:$Z$279,1),1)</f>
+        <v>CTL1</v>
+      </c>
+    </row>
+    <row r="269" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B269" s="43">
         <v>106</v>
       </c>
@@ -10303,8 +10506,29 @@
       <c r="P269" s="38" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="270" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U269" s="66" t="str">
+        <v>DBM2</v>
+      </c>
+      <c r="V269" s="66" t="str">
+        <v>Dry Bulk</v>
+      </c>
+      <c r="W269" s="66">
+        <v>80000</v>
+      </c>
+      <c r="X269" s="11" t="str">
+        <f ca="1"/>
+        <v>CTS1</v>
+      </c>
+      <c r="Y269" s="11">
+        <f ca="1"/>
+        <v>1000</v>
+      </c>
+      <c r="Z269" s="11">
+        <f ca="1">SUM($Y$268:Y269)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="270" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B270" s="43">
         <v>107</v>
       </c>
@@ -10346,8 +10570,29 @@
       <c r="P270" s="38" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="271" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U270" s="66" t="str">
+        <v>LBL2</v>
+      </c>
+      <c r="V270" s="66" t="str">
+        <v>Liquid Bulk</v>
+      </c>
+      <c r="W270" s="66">
+        <v>150000</v>
+      </c>
+      <c r="X270" s="11" t="str">
+        <f ca="1"/>
+        <v>CTL1</v>
+      </c>
+      <c r="Y270" s="11">
+        <f ca="1"/>
+        <v>12000</v>
+      </c>
+      <c r="Z270" s="11">
+        <f ca="1">SUM($Y$268:Y270)</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="271" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B271" s="43">
         <v>108</v>
       </c>
@@ -10389,8 +10634,29 @@
       <c r="P271" s="38" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="272" spans="2:16" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="U271" s="66" t="str">
+        <v>DBL2</v>
+      </c>
+      <c r="V271" s="66" t="str">
+        <v>Dry Bulk</v>
+      </c>
+      <c r="W271" s="66">
+        <v>185000</v>
+      </c>
+      <c r="X271" s="11" t="str">
+        <f ca="1"/>
+        <v>CTL2</v>
+      </c>
+      <c r="Y271" s="11">
+        <f ca="1"/>
+        <v>20000</v>
+      </c>
+      <c r="Z271" s="11">
+        <f ca="1">SUM($Y$268:Y271)</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="272" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B272" s="43">
         <v>109</v>
       </c>
@@ -10432,6 +10698,19 @@
       <c r="P272" s="38" t="s">
         <v>174</v>
       </c>
+      <c r="U272" s="66" t="str">
+        <v>DBM1</v>
+      </c>
+      <c r="V272" s="66" t="str">
+        <v>Dry Bulk</v>
+      </c>
+      <c r="W272" s="66">
+        <v>60000</v>
+      </c>
+      <c r="Z272" s="11">
+        <f ca="1">SUM($Y$268:Y272)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="273" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B273" s="43">
@@ -10475,6 +10754,19 @@
       <c r="P273" s="38" t="s">
         <v>175</v>
       </c>
+      <c r="U273" s="66" t="str">
+        <v>LBM2</v>
+      </c>
+      <c r="V273" s="66" t="str">
+        <v>Liquid Bulk</v>
+      </c>
+      <c r="W273" s="66">
+        <v>75000</v>
+      </c>
+      <c r="Z273" s="11">
+        <f ca="1">SUM($Y$268:Y273)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="274" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B274" s="43">
@@ -10518,6 +10810,19 @@
       <c r="P274" s="38" t="s">
         <v>176</v>
       </c>
+      <c r="U274" s="66" t="str">
+        <v>CTS2</v>
+      </c>
+      <c r="V274" s="66" t="str">
+        <v>Container</v>
+      </c>
+      <c r="W274" s="66">
+        <v>2000</v>
+      </c>
+      <c r="Z274" s="11">
+        <f ca="1">SUM($Y$268:Y274)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="275" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B275" s="43">
@@ -10561,6 +10866,19 @@
       <c r="P275" s="38" t="s">
         <v>177</v>
       </c>
+      <c r="U275" s="66" t="str">
+        <v>LBM1</v>
+      </c>
+      <c r="V275" s="66" t="str">
+        <v>Liquid Bulk</v>
+      </c>
+      <c r="W275" s="66">
+        <v>50000</v>
+      </c>
+      <c r="Z275" s="11">
+        <f ca="1">SUM($Y$268:Y275)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="276" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B276" s="43">
@@ -10604,6 +10922,19 @@
       <c r="P276" s="38" t="s">
         <v>178</v>
       </c>
+      <c r="U276" s="66" t="str">
+        <v>CTS1</v>
+      </c>
+      <c r="V276" s="66" t="str">
+        <v>Container</v>
+      </c>
+      <c r="W276" s="66">
+        <v>1000</v>
+      </c>
+      <c r="Z276" s="11">
+        <f ca="1">SUM($Y$268:Y276)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="277" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B277" s="43">
@@ -10647,6 +10978,19 @@
       <c r="P277" s="38" t="s">
         <v>179</v>
       </c>
+      <c r="U277" s="66" t="str">
+        <v>CTL1</v>
+      </c>
+      <c r="V277" s="66" t="str">
+        <v>Container</v>
+      </c>
+      <c r="W277" s="66">
+        <v>12000</v>
+      </c>
+      <c r="Z277" s="11">
+        <f ca="1">SUM($Y$268:Y277)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="278" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B278" s="43">
@@ -10690,6 +11034,19 @@
       <c r="P278" s="38" t="s">
         <v>180</v>
       </c>
+      <c r="U278" s="66" t="str">
+        <v>LBL3</v>
+      </c>
+      <c r="V278" s="66" t="str">
+        <v>Liquid Bulk</v>
+      </c>
+      <c r="W278" s="66">
+        <v>200000</v>
+      </c>
+      <c r="Z278" s="11">
+        <f ca="1">SUM($Y$268:Y278)</f>
+        <v>35000</v>
+      </c>
     </row>
     <row r="279" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B279" s="43">
@@ -10732,6 +11089,19 @@
       </c>
       <c r="P279" s="38" t="s">
         <v>181</v>
+      </c>
+      <c r="U279" s="70" t="str">
+        <v>CTL2</v>
+      </c>
+      <c r="V279" s="70" t="str">
+        <v>Container</v>
+      </c>
+      <c r="W279" s="70">
+        <v>20000</v>
+      </c>
+      <c r="Z279" s="11">
+        <f ca="1">SUM($Y$268:Y279)</f>
+        <v>35000</v>
       </c>
     </row>
     <row r="280" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
@@ -10938,7 +11308,7 @@
       <c r="R285" s="1"/>
       <c r="S285" s="1"/>
       <c r="T285" s="1"/>
-      <c r="U285" s="1"/>
+      <c r="U285" s="11"/>
       <c r="V285" s="1"/>
       <c r="W285" s="1"/>
       <c r="X285" s="1"/>
@@ -10949,6 +11319,7 @@
     <row r="286" spans="1:27" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="F286" s="20"/>
       <c r="K286" s="45"/>
+      <c r="U286" s="1"/>
     </row>
     <row r="287" spans="1:27" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="F287" s="20"/>
@@ -10970,6 +11341,7 @@
       <c r="N288" s="11"/>
       <c r="O288" s="11"/>
       <c r="P288" s="11"/>
+      <c r="U288" s="11"/>
     </row>
     <row r="289" spans="2:16">
       <c r="B289" s="11"/>
@@ -11308,7 +11680,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:F26"/>
     </sheetView>
   </sheetViews>
@@ -11323,15 +11695,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="84"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="92"/>
     </row>
     <row r="2" spans="1:7" ht="16.95" customHeight="1">
       <c r="A2" s="60" t="s">
@@ -11936,11 +12308,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.95" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="90" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" ht="16.8" customHeight="1">
       <c r="A2" s="60" t="s">
@@ -12184,19 +12556,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.95" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="84"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="92"/>
     </row>
     <row r="2" spans="1:4" ht="16.95" customHeight="1">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="93" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="86"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3" spans="1:4" ht="16.95" customHeight="1">
       <c r="A3" s="63" t="s">
@@ -12383,8 +12755,8 @@
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:AA289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B213" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+    <sheetView topLeftCell="K255" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W268" sqref="W268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -12404,46 +12776,46 @@
     <col min="20" max="20" width="9.3984375" style="1" customWidth="1"/>
     <col min="21" max="21" width="8.3984375" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.796875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="4.796875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10.09765625" style="1" customWidth="1"/>
     <col min="24" max="24" width="16.09765625" style="1" customWidth="1"/>
     <col min="25" max="16384" width="15.8984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1"/>
     <row r="2" spans="2:13" ht="59.25" customHeight="1">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="75"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1"/>
     <row r="4" spans="2:13" ht="33" customHeight="1">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="70"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="2:13" ht="196.2" customHeight="1">
       <c r="C5"/>
@@ -12454,10 +12826,10 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:13" ht="33" customHeight="1">
-      <c r="L6" s="68" t="s">
+      <c r="L6" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="70"/>
+      <c r="M6" s="78"/>
     </row>
     <row r="7" spans="2:13" ht="113.4" customHeight="1">
       <c r="K7" s="4"/>
@@ -12465,52 +12837,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
     </row>
     <row r="9" spans="2:13" ht="81" customHeight="1">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="2:13" ht="189.6" customHeight="1">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1">
       <c r="B11" s="6"/>
@@ -12527,20 +12899,20 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="70"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="78"/>
     </row>
     <row r="13" spans="2:13" ht="15" customHeight="1">
       <c r="B13" s="8"/>
@@ -12590,15 +12962,15 @@
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="78" t="s">
+      <c r="G16" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="80"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="88"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="17" t="s">
@@ -12617,15 +12989,15 @@
         <f>IF(ISBLANK(Case!E17), 0, IF(E17=Case!E17, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="81" t="s">
+      <c r="G17" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="17" t="s">
@@ -12644,15 +13016,15 @@
         <f>IF(ISBLANK(Case!E18), 0, IF(E18=Case!E18, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="G18" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="17" t="s">
@@ -12671,15 +13043,15 @@
         <f>IF(ISBLANK(Case!E19), 0, IF(E19=Case!E19, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="17" t="s">
@@ -12698,15 +13070,15 @@
         <f>IF(ISBLANK(Case!E20), 0, IF(E20=Case!E20, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G20" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="17" t="s">
@@ -12725,34 +13097,34 @@
         <f>IF(ISBLANK(Case!E21), 0, IF(E21=Case!E21, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="74" t="s">
+      <c r="G21" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="76"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="84"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.4">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="70"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="78"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="24"/>
@@ -12778,21 +13150,21 @@
       <c r="D25" s="20"/>
       <c r="E25" s="28"/>
       <c r="F25" s="20"/>
-      <c r="L25" s="68" t="s">
+      <c r="L25" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="M25" s="70"/>
+      <c r="M25" s="78"/>
     </row>
     <row r="26" spans="2:13" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B26" s="29"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
-      <c r="L26" s="87">
+      <c r="L26" s="95">
         <f>SUMPRODUCT(--(F17:F338=1),D17:D338)</f>
         <v>760</v>
       </c>
-      <c r="M26" s="88"/>
+      <c r="M26" s="96"/>
     </row>
     <row r="27" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B27" s="28" t="s">
@@ -12802,8 +13174,8 @@
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="90"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="98"/>
     </row>
     <row r="28" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B28" s="30"/>
@@ -12811,8 +13183,8 @@
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="L28" s="91"/>
-      <c r="M28" s="92"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="100"/>
     </row>
     <row r="29" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B29" s="31" t="s">

</xml_diff>

<commit_message>
Updated hard problem. Almost got it
</commit_message>
<xml_diff>
--- a/2025 Excel Esports Chille - The Docks of Valparaiso (Juan Jose Cifuentes) - Case and Answers.xlsx
+++ b/2025 Excel Esports Chille - The Docks of Valparaiso (Juan Jose Cifuentes) - Case and Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A512AB-2A44-4366-8A42-908FA8AAC5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0506AA6-BA04-4A29-B758-A10108D144E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE4A18CD-9E80-4D14-A39F-1C9BD96D766A}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="238">
   <si>
     <t>Juan José Cifuentes</t>
   </si>
@@ -781,6 +781,21 @@
   </si>
   <si>
     <t>Cargo 1</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Cumulative</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Goods</t>
+  </si>
+  <si>
+    <t>Almost got it. I did not get the partially full ship.</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1321,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1509,33 +1524,6 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1547,6 +1535,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1562,6 +1559,24 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1595,6 +1610,15 @@
     </xf>
     <xf numFmtId="3" fontId="27" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2924,10 +2948,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E46771-3E32-4515-837B-D61C1E8E2229}">
   <sheetPr codeName="Sheet28"/>
-  <dimension ref="A1:AA289"/>
+  <dimension ref="A1:AE292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P266" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S272" sqref="S272"/>
+    <sheetView tabSelected="1" topLeftCell="S260" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z268" sqref="Z268:Z271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -2950,20 +2974,20 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1"/>
     <row r="2" spans="2:13" ht="59.25" customHeight="1">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="75"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1"/>
     <row r="4" spans="2:13" ht="33" customHeight="1">
@@ -3004,52 +3028,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
     </row>
     <row r="9" spans="2:13" ht="79.2" customHeight="1">
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
     </row>
     <row r="10" spans="2:13" ht="194.4" customHeight="1">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="85"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1">
       <c r="B11" s="5"/>
@@ -3129,15 +3153,15 @@
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="86" t="s">
+      <c r="G16" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="88"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="82"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="16" t="s">
@@ -3151,15 +3175,15 @@
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="89" t="s">
+      <c r="G17" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="89"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="16" t="s">
@@ -3173,15 +3197,15 @@
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="81" t="s">
+      <c r="G18" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="16" t="s">
@@ -3195,15 +3219,15 @@
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="81" t="s">
+      <c r="G19" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="16" t="s">
@@ -3217,15 +3241,15 @@
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="81" t="s">
+      <c r="G20" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="16" t="s">
@@ -3239,15 +3263,15 @@
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="84"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="75"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
@@ -9981,7 +10005,7 @@
       <c r="F256" s="20"/>
       <c r="G256" s="28"/>
     </row>
-    <row r="257" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="257" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B257" s="32" t="s">
         <v>160</v>
       </c>
@@ -9990,8 +10014,11 @@
       <c r="E257" s="20"/>
       <c r="F257" s="20"/>
       <c r="G257" s="28"/>
-    </row>
-    <row r="258" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1">
+      <c r="Z257" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="258" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B258" s="32" t="s">
         <v>161</v>
       </c>
@@ -10001,7 +10028,7 @@
       <c r="F258" s="20"/>
       <c r="G258" s="28"/>
     </row>
-    <row r="259" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="259" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="B259" s="29"/>
       <c r="C259" s="20"/>
       <c r="D259" s="20"/>
@@ -10009,7 +10036,7 @@
       <c r="F259" s="20"/>
       <c r="G259" s="28"/>
     </row>
-    <row r="260" spans="2:27" s="11" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
+    <row r="260" spans="2:31" s="11" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
       <c r="B260" s="13" t="s">
         <v>10</v>
       </c>
@@ -10057,10 +10084,25 @@
         <v>229</v>
       </c>
       <c r="V260" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
+        <v>8</v>
+      </c>
+      <c r="Z260" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AB260" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC260" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD260" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE260" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="261" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="F261" s="20"/>
       <c r="U261" s="67" t="s">
         <v>53</v>
@@ -10075,8 +10117,32 @@
         <v>230</v>
       </c>
       <c r="Y261"/>
-    </row>
-    <row r="262" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
+      <c r="Z261" s="11" t="str" cm="1">
+        <f t="array" ref="Z261">INDEX($O$262:$O$283,V260)</f>
+        <v>Iron Ore</v>
+      </c>
+      <c r="AA261" s="11" t="str">
+        <f>_xlfn.XLOOKUP(Z261,_tCList[Cargo],_tCList[Cargo Type])</f>
+        <v>Dry Bulk</v>
+      </c>
+      <c r="AB261" s="11" t="str" cm="1">
+        <f t="array" aca="1" ref="AB261:AD262" ca="1">_xlfn.LET(_xlpm.z,_xlfn._xlws.FILTER(_xlfn.HSTACK($U$262:$U$265,$X$262:$X$265,$V$262:$V$265),$W$262:$W$265=AA261),_xlfn._xlws.SORT(_xlpm.z,2,-1))</f>
+        <v>Cellulose</v>
+      </c>
+      <c r="AC261" s="11">
+        <f ca="1"/>
+        <v>500</v>
+      </c>
+      <c r="AD261" s="11">
+        <f ca="1"/>
+        <v>115600.00000000001</v>
+      </c>
+      <c r="AE261" s="11" cm="1">
+        <f t="array" aca="1" ref="AE261:AE262" ca="1">_xlfn.SCAN(0,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(AB261),3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v))</f>
+        <v>115600.00000000001</v>
+      </c>
+    </row>
+    <row r="262" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
       <c r="B262" s="35" t="s">
         <v>164</v>
       </c>
@@ -10122,25 +10188,38 @@
       </c>
       <c r="U262" s="68" t="str" cm="1">
         <f t="array" aca="1" ref="U262:V262" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U262)*2-2,$V$260,2),$V$260,)</f>
-        <v>Cellulose</v>
+        <v>Sulfuric Acid</v>
       </c>
       <c r="V262" s="66">
         <f ca="1"/>
-        <v>68400</v>
+        <v>122400.00000000001</v>
       </c>
       <c r="W262" s="66" t="str">
         <f ca="1">_xlfn.XLOOKUP(U262,_tCList[Cargo],_tCList[Cargo Type])</f>
-        <v>Dry Bulk</v>
+        <v>Liquid Bulk</v>
       </c>
       <c r="X262" s="66">
         <f ca="1">_xlfn.XLOOKUP(U262,_tCList[Cargo],_tCList[Value per Unit])</f>
-        <v>500</v>
-      </c>
-      <c r="AA262" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="263" spans="2:27" s="11" customFormat="1" ht="15" customHeight="1">
+        <v>150</v>
+      </c>
+      <c r="AB262" s="11" t="str">
+        <f ca="1"/>
+        <v>Iron Ore</v>
+      </c>
+      <c r="AC262" s="11">
+        <f ca="1"/>
+        <v>150</v>
+      </c>
+      <c r="AD262" s="11">
+        <f ca="1"/>
+        <v>91800</v>
+      </c>
+      <c r="AE262" s="11">
+        <f ca="1"/>
+        <v>207400</v>
+      </c>
+    </row>
+    <row r="263" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="E263" s="40"/>
       <c r="F263" s="20"/>
       <c r="G263" s="41"/>
@@ -10155,25 +10234,22 @@
       <c r="P263" s="41"/>
       <c r="U263" s="68" t="str" cm="1">
         <f t="array" aca="1" ref="U263:V263" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U263)*2-2,$V$260,2),$V$260,)</f>
-        <v>Sulfuric Acid</v>
+        <v>Iron Ore</v>
       </c>
       <c r="V263" s="66">
         <f ca="1"/>
-        <v>7200</v>
+        <v>91800</v>
       </c>
       <c r="W263" s="66" t="str">
         <f ca="1">_xlfn.XLOOKUP(U263,_tCList[Cargo],_tCList[Cargo Type])</f>
-        <v>Liquid Bulk</v>
+        <v>Dry Bulk</v>
       </c>
       <c r="X263" s="66">
         <f ca="1">_xlfn.XLOOKUP(U263,_tCList[Cargo],_tCList[Value per Unit])</f>
         <v>150</v>
       </c>
-      <c r="AA263" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="264" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+    </row>
+    <row r="264" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B264" s="43">
         <v>101</v>
       </c>
@@ -10183,7 +10259,9 @@
       <c r="D264" s="44">
         <v>12</v>
       </c>
-      <c r="E264" s="19"/>
+      <c r="E264" s="19">
+        <v>6</v>
+      </c>
       <c r="F264" s="20"/>
       <c r="G264" s="38" t="s">
         <v>145</v>
@@ -10217,11 +10295,11 @@
       </c>
       <c r="U264" s="68" t="str" cm="1">
         <f t="array" aca="1" ref="U264:V264" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U264)*2-2,$V$260,2),$V$260,)</f>
-        <v>Salmon</v>
+        <v>Blueberries</v>
       </c>
       <c r="V264" s="66">
         <f ca="1"/>
-        <v>5760</v>
+        <v>1020.0000000000001</v>
       </c>
       <c r="W264" s="66" t="str">
         <f ca="1">_xlfn.XLOOKUP(U264,_tCList[Cargo],_tCList[Cargo Type])</f>
@@ -10229,13 +10307,10 @@
       </c>
       <c r="X264" s="66">
         <f ca="1">_xlfn.XLOOKUP(U264,_tCList[Cargo],_tCList[Value per Unit])</f>
-        <v>120000</v>
-      </c>
-      <c r="AA264" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="265" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="265" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B265" s="43">
         <v>102</v>
       </c>
@@ -10245,7 +10320,9 @@
       <c r="D265" s="44">
         <v>12</v>
       </c>
-      <c r="E265" s="19"/>
+      <c r="E265" s="19">
+        <v>1</v>
+      </c>
       <c r="F265" s="20"/>
       <c r="G265" s="38" t="s">
         <v>64</v>
@@ -10279,11 +10356,11 @@
       </c>
       <c r="U265" s="69" t="str" cm="1">
         <f t="array" aca="1" ref="U265:V265" ca="1">INDEX(OFFSET($G$262:$I$283,0,ROWS($U$262:U265)*2-2,$V$260,2),$V$260,)</f>
-        <v>Iron Ore</v>
+        <v>Cellulose</v>
       </c>
       <c r="V265" s="70">
         <f ca="1"/>
-        <v>82800</v>
+        <v>115600.00000000001</v>
       </c>
       <c r="W265" s="70" t="str">
         <f ca="1">_xlfn.XLOOKUP(U265,_tCList[Cargo],_tCList[Cargo Type])</f>
@@ -10291,10 +10368,22 @@
       </c>
       <c r="X265" s="70">
         <f ca="1">_xlfn.XLOOKUP(U265,_tCList[Cargo],_tCList[Value per Unit])</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="266" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>500</v>
+      </c>
+      <c r="AB265" s="11" cm="1">
+        <f t="array" aca="1" ref="AB265" ca="1">_xlfn.XLOOKUP(Z261,_xlfn.TAKE(_xlfn.ANCHORARRAY(AB261),,1),_xlfn.ANCHORARRAY(AE261))</f>
+        <v>207400</v>
+      </c>
+      <c r="AC265" s="11" t="str" cm="1">
+        <f t="array" aca="1" ref="AC265" ca="1">_xlfn.XLOOKUP(AB265,_xlfn.ANCHORARRAY(Z268),_xlfn.TAKE(_xlfn.ANCHORARRAY(X268),,1),,1)</f>
+        <v>DBL4</v>
+      </c>
+      <c r="AD265" s="11">
+        <f ca="1">_xlfn.IFNA(_xlfn.XMATCH(AC265,_xlfn.ANCHORARRAY(U268)),"X")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B266" s="43">
         <v>103</v>
       </c>
@@ -10304,7 +10393,9 @@
       <c r="D266" s="44">
         <v>12</v>
       </c>
-      <c r="E266" s="19"/>
+      <c r="E266" s="19" t="s">
+        <v>224</v>
+      </c>
       <c r="F266" s="20"/>
       <c r="G266" s="38" t="s">
         <v>61</v>
@@ -10337,7 +10428,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="267" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="267" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
       <c r="B267" s="43">
         <v>104</v>
       </c>
@@ -10347,7 +10438,9 @@
       <c r="D267" s="44">
         <v>12</v>
       </c>
-      <c r="E267" s="19"/>
+      <c r="E267" s="19">
+        <v>11</v>
+      </c>
       <c r="F267" s="20"/>
       <c r="G267" s="38" t="s">
         <v>60</v>
@@ -10393,7 +10486,7 @@
       </c>
       <c r="Z267"/>
     </row>
-    <row r="268" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
+    <row r="268" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
       <c r="B268" s="43">
         <v>105</v>
       </c>
@@ -10403,7 +10496,9 @@
       <c r="D268" s="44">
         <v>12</v>
       </c>
-      <c r="E268" s="19"/>
+      <c r="E268" s="19">
+        <v>7</v>
+      </c>
       <c r="F268" s="20"/>
       <c r="G268" s="38" t="s">
         <v>145</v>
@@ -10437,34 +10532,29 @@
       </c>
       <c r="U268" s="66" t="str" cm="1">
         <f t="array" ref="U268:U279">_xlfn.TEXTSPLIT(INDEX($P$262:$P$283,V260),,";")</f>
-        <v>DBS3</v>
+        <v>LBS1</v>
       </c>
       <c r="V268" s="66" t="str" cm="1">
         <f t="array" ref="V268:V279">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(U268),_tCapacity[Model ID],_tCapacity[Cargo Type])</f>
-        <v>Dry Bulk</v>
+        <v>Liquid Bulk</v>
       </c>
       <c r="W268" s="66" cm="1">
         <f t="array" ref="W268:W279">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(U268),_tCapacity[Model ID],_tCapacity[Capacity])</f>
-        <v>35000</v>
+        <v>5000</v>
       </c>
       <c r="X268" s="11" t="str" cm="1">
-        <f t="array" aca="1" ref="X268:Y271" ca="1">_xlfn._xlws.FILTER(_xlfn.HSTACK(_xlfn.ANCHORARRAY(U268),_xlfn.ANCHORARRAY(W268)),_xlfn.ANCHORARRAY(V268)=W264)</f>
-        <v>CTS2</v>
+        <f t="array" ref="X268:Y271">_xlfn._xlws.FILTER(_xlfn.HSTACK(_xlfn.ANCHORARRAY(U268),_xlfn.ANCHORARRAY(W268)),_xlfn.ANCHORARRAY(V268)=$AA$261)</f>
+        <v>DBM2</v>
       </c>
       <c r="Y268" s="11">
-        <f ca="1"/>
-        <v>2000</v>
-      </c>
-      <c r="Z268" s="11">
-        <f ca="1">SUM($Y$268:Y268)</f>
-        <v>2000</v>
-      </c>
-      <c r="AA268" s="11" t="str" cm="1">
-        <f t="array" aca="1" ref="AA268" ca="1">INDEX(_xlfn.ANCHORARRAY(X268),_xlfn.XMATCH(V264,$Z$268:$Z$279,1),1)</f>
-        <v>CTL1</v>
-      </c>
-    </row>
-    <row r="269" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>80000</v>
+      </c>
+      <c r="Z268" s="11" cm="1">
+        <f t="array" ref="Z268:Z271">_xlfn.SCAN(0,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(X268),2),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,SUM(_xlpm.a+_xlpm.v)))</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="269" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B269" s="43">
         <v>106</v>
       </c>
@@ -10474,7 +10564,9 @@
       <c r="D269" s="44">
         <v>12</v>
       </c>
-      <c r="E269" s="19"/>
+      <c r="E269" s="19">
+        <v>7</v>
+      </c>
       <c r="F269" s="20"/>
       <c r="G269" s="38" t="s">
         <v>63</v>
@@ -10516,19 +10608,16 @@
         <v>80000</v>
       </c>
       <c r="X269" s="11" t="str">
-        <f ca="1"/>
-        <v>CTS1</v>
+        <v>DBL4</v>
       </c>
       <c r="Y269" s="11">
-        <f ca="1"/>
-        <v>1000</v>
+        <v>220000</v>
       </c>
       <c r="Z269" s="11">
-        <f ca="1">SUM($Y$268:Y269)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="270" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="270" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B270" s="43">
         <v>107</v>
       </c>
@@ -10538,7 +10627,9 @@
       <c r="D270" s="44">
         <v>12</v>
       </c>
-      <c r="E270" s="19"/>
+      <c r="E270" s="19">
+        <v>9</v>
+      </c>
       <c r="F270" s="20"/>
       <c r="G270" s="38" t="s">
         <v>145</v>
@@ -10571,28 +10662,25 @@
         <v>172</v>
       </c>
       <c r="U270" s="66" t="str">
-        <v>LBL2</v>
+        <v>LBL3</v>
       </c>
       <c r="V270" s="66" t="str">
         <v>Liquid Bulk</v>
       </c>
       <c r="W270" s="66">
-        <v>150000</v>
+        <v>200000</v>
       </c>
       <c r="X270" s="11" t="str">
-        <f ca="1"/>
-        <v>CTL1</v>
+        <v>DBS3</v>
       </c>
       <c r="Y270" s="11">
-        <f ca="1"/>
-        <v>12000</v>
+        <v>35000</v>
       </c>
       <c r="Z270" s="11">
-        <f ca="1">SUM($Y$268:Y270)</f>
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="271" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>335000</v>
+      </c>
+    </row>
+    <row r="271" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B271" s="43">
         <v>108</v>
       </c>
@@ -10602,7 +10690,9 @@
       <c r="D271" s="44">
         <v>12</v>
       </c>
-      <c r="E271" s="19"/>
+      <c r="E271" s="19">
+        <v>3</v>
+      </c>
       <c r="F271" s="20"/>
       <c r="G271" s="38" t="s">
         <v>63</v>
@@ -10635,28 +10725,25 @@
         <v>173</v>
       </c>
       <c r="U271" s="66" t="str">
-        <v>DBL2</v>
+        <v>CTM2</v>
       </c>
       <c r="V271" s="66" t="str">
-        <v>Dry Bulk</v>
+        <v>Container</v>
       </c>
       <c r="W271" s="66">
-        <v>185000</v>
+        <v>7000</v>
       </c>
       <c r="X271" s="11" t="str">
-        <f ca="1"/>
-        <v>CTL2</v>
+        <v>DBM1</v>
       </c>
       <c r="Y271" s="11">
-        <f ca="1"/>
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="Z271" s="11">
-        <f ca="1">SUM($Y$268:Y271)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="272" spans="2:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>395000</v>
+      </c>
+    </row>
+    <row r="272" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B272" s="43">
         <v>109</v>
       </c>
@@ -10666,7 +10753,9 @@
       <c r="D272" s="44">
         <v>12</v>
       </c>
-      <c r="E272" s="19"/>
+      <c r="E272" s="19">
+        <v>2</v>
+      </c>
       <c r="F272" s="20"/>
       <c r="G272" s="38" t="s">
         <v>59</v>
@@ -10699,20 +10788,20 @@
         <v>174</v>
       </c>
       <c r="U272" s="66" t="str">
-        <v>DBM1</v>
+        <v>LBL1</v>
       </c>
       <c r="V272" s="66" t="str">
-        <v>Dry Bulk</v>
+        <v>Liquid Bulk</v>
       </c>
       <c r="W272" s="66">
-        <v>60000</v>
-      </c>
-      <c r="Z272" s="11">
-        <f ca="1">SUM($Y$268:Y272)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="273" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>100000</v>
+      </c>
+      <c r="AB272" s="11">
+        <f ca="1">AD265</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B273" s="43">
         <v>110</v>
       </c>
@@ -10722,7 +10811,9 @@
       <c r="D273" s="44">
         <v>12</v>
       </c>
-      <c r="E273" s="19"/>
+      <c r="E273" s="19" t="s">
+        <v>224</v>
+      </c>
       <c r="F273" s="20"/>
       <c r="G273" s="38" t="s">
         <v>146</v>
@@ -10755,20 +10846,24 @@
         <v>175</v>
       </c>
       <c r="U273" s="66" t="str">
-        <v>LBM2</v>
+        <v>CTM1</v>
       </c>
       <c r="V273" s="66" t="str">
-        <v>Liquid Bulk</v>
+        <v>Container</v>
       </c>
       <c r="W273" s="66">
-        <v>75000</v>
-      </c>
-      <c r="Z273" s="11">
-        <f ca="1">SUM($Y$268:Y273)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="274" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>4500</v>
+      </c>
+      <c r="AA273" s="11" cm="1">
+        <f t="array" ref="AA273:AA292">_xlfn.SEQUENCE(20,1,3)</f>
+        <v>3</v>
+      </c>
+      <c r="AB273" s="101">
+        <f t="dataTable" ref="AB273:AB292" dt2D="0" dtr="0" r1="V260" ca="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B274" s="43">
         <v>111</v>
       </c>
@@ -10778,7 +10873,9 @@
       <c r="D274" s="44">
         <v>12</v>
       </c>
-      <c r="E274" s="19"/>
+      <c r="E274" s="19" t="s">
+        <v>224</v>
+      </c>
       <c r="F274" s="20"/>
       <c r="G274" s="38" t="s">
         <v>58</v>
@@ -10811,20 +10908,22 @@
         <v>176</v>
       </c>
       <c r="U274" s="66" t="str">
-        <v>CTS2</v>
+        <v>DBL4</v>
       </c>
       <c r="V274" s="66" t="str">
-        <v>Container</v>
+        <v>Dry Bulk</v>
       </c>
       <c r="W274" s="66">
-        <v>2000</v>
-      </c>
-      <c r="Z274" s="11">
-        <f ca="1">SUM($Y$268:Y274)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="275" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>220000</v>
+      </c>
+      <c r="AA274" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB274" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B275" s="43">
         <v>112</v>
       </c>
@@ -10834,7 +10933,9 @@
       <c r="D275" s="44">
         <v>12</v>
       </c>
-      <c r="E275" s="19"/>
+      <c r="E275" s="19">
+        <v>5</v>
+      </c>
       <c r="F275" s="20"/>
       <c r="G275" s="38" t="s">
         <v>57</v>
@@ -10867,20 +10968,22 @@
         <v>177</v>
       </c>
       <c r="U275" s="66" t="str">
-        <v>LBM1</v>
+        <v>CTS1</v>
       </c>
       <c r="V275" s="66" t="str">
-        <v>Liquid Bulk</v>
+        <v>Container</v>
       </c>
       <c r="W275" s="66">
-        <v>50000</v>
-      </c>
-      <c r="Z275" s="11">
-        <f ca="1">SUM($Y$268:Y275)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="276" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>1000</v>
+      </c>
+      <c r="AA275" s="11">
+        <v>5</v>
+      </c>
+      <c r="AB275" s="101" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="276" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B276" s="43">
         <v>113</v>
       </c>
@@ -10890,7 +10993,9 @@
       <c r="D276" s="44">
         <v>12</v>
       </c>
-      <c r="E276" s="19"/>
+      <c r="E276" s="19" t="s">
+        <v>224</v>
+      </c>
       <c r="F276" s="20"/>
       <c r="G276" s="38" t="s">
         <v>60</v>
@@ -10923,20 +11028,22 @@
         <v>178</v>
       </c>
       <c r="U276" s="66" t="str">
-        <v>CTS1</v>
+        <v>CTL1</v>
       </c>
       <c r="V276" s="66" t="str">
         <v>Container</v>
       </c>
       <c r="W276" s="66">
-        <v>1000</v>
-      </c>
-      <c r="Z276" s="11">
-        <f ca="1">SUM($Y$268:Y276)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="277" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>12000</v>
+      </c>
+      <c r="AA276" s="11">
+        <v>6</v>
+      </c>
+      <c r="AB276" s="101">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="277" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B277" s="43">
         <v>114</v>
       </c>
@@ -10946,7 +11053,9 @@
       <c r="D277" s="44">
         <v>12</v>
       </c>
-      <c r="E277" s="19"/>
+      <c r="E277" s="19" t="s">
+        <v>224</v>
+      </c>
       <c r="F277" s="20"/>
       <c r="G277" s="38" t="s">
         <v>57</v>
@@ -10979,20 +11088,22 @@
         <v>179</v>
       </c>
       <c r="U277" s="66" t="str">
-        <v>CTL1</v>
+        <v>LBL4</v>
       </c>
       <c r="V277" s="66" t="str">
-        <v>Container</v>
+        <v>Liquid Bulk</v>
       </c>
       <c r="W277" s="66">
-        <v>12000</v>
-      </c>
-      <c r="Z277" s="11">
-        <f ca="1">SUM($Y$268:Y277)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="278" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>300000</v>
+      </c>
+      <c r="AA277" s="11">
+        <v>7</v>
+      </c>
+      <c r="AB277" s="101">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="278" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B278" s="43">
         <v>115</v>
       </c>
@@ -11002,7 +11113,9 @@
       <c r="D278" s="44">
         <v>12</v>
       </c>
-      <c r="E278" s="19"/>
+      <c r="E278" s="19" t="s">
+        <v>224</v>
+      </c>
       <c r="F278" s="20"/>
       <c r="G278" s="38" t="s">
         <v>146</v>
@@ -11035,20 +11148,22 @@
         <v>180</v>
       </c>
       <c r="U278" s="66" t="str">
-        <v>LBL3</v>
+        <v>DBS3</v>
       </c>
       <c r="V278" s="66" t="str">
-        <v>Liquid Bulk</v>
+        <v>Dry Bulk</v>
       </c>
       <c r="W278" s="66">
-        <v>200000</v>
-      </c>
-      <c r="Z278" s="11">
-        <f ca="1">SUM($Y$268:Y278)</f>
         <v>35000</v>
       </c>
-    </row>
-    <row r="279" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="AA278" s="11">
+        <v>8</v>
+      </c>
+      <c r="AB278" s="101">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B279" s="43">
         <v>116</v>
       </c>
@@ -11058,7 +11173,9 @@
       <c r="D279" s="44">
         <v>12</v>
       </c>
-      <c r="E279" s="19"/>
+      <c r="E279" s="19">
+        <v>5</v>
+      </c>
       <c r="F279" s="20"/>
       <c r="G279" s="38" t="s">
         <v>62</v>
@@ -11091,20 +11208,22 @@
         <v>181</v>
       </c>
       <c r="U279" s="70" t="str">
-        <v>CTL2</v>
+        <v>DBM1</v>
       </c>
       <c r="V279" s="70" t="str">
-        <v>Container</v>
+        <v>Dry Bulk</v>
       </c>
       <c r="W279" s="70">
-        <v>20000</v>
-      </c>
-      <c r="Z279" s="11">
-        <f ca="1">SUM($Y$268:Y279)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="280" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+        <v>60000</v>
+      </c>
+      <c r="AA279" s="11">
+        <v>9</v>
+      </c>
+      <c r="AB279" s="101">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="280" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B280" s="43">
         <v>117</v>
       </c>
@@ -11114,7 +11233,9 @@
       <c r="D280" s="44">
         <v>12</v>
       </c>
-      <c r="E280" s="19"/>
+      <c r="E280" s="19">
+        <v>2</v>
+      </c>
       <c r="F280" s="20"/>
       <c r="G280" s="38" t="s">
         <v>59</v>
@@ -11146,8 +11267,14 @@
       <c r="P280" s="38" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="281" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="AA280" s="11">
+        <v>10</v>
+      </c>
+      <c r="AB280" s="101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B281" s="43">
         <v>118</v>
       </c>
@@ -11157,7 +11284,9 @@
       <c r="D281" s="44">
         <v>12</v>
       </c>
-      <c r="E281" s="19"/>
+      <c r="E281" s="19">
+        <v>4</v>
+      </c>
       <c r="F281" s="20"/>
       <c r="G281" s="38" t="s">
         <v>147</v>
@@ -11189,8 +11318,14 @@
       <c r="P281" s="38" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="282" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="AA281" s="11">
+        <v>11</v>
+      </c>
+      <c r="AB281" s="101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B282" s="43">
         <v>119</v>
       </c>
@@ -11200,7 +11335,9 @@
       <c r="D282" s="44">
         <v>12</v>
       </c>
-      <c r="E282" s="19"/>
+      <c r="E282" s="19">
+        <v>5</v>
+      </c>
       <c r="F282" s="20"/>
       <c r="G282" s="38" t="s">
         <v>64</v>
@@ -11232,8 +11369,14 @@
       <c r="P282" s="38" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="283" spans="1:27" s="11" customFormat="1" ht="23.25" customHeight="1">
+      <c r="AA282" s="11">
+        <v>12</v>
+      </c>
+      <c r="AB282" s="101" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="283" spans="1:28" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B283" s="43">
         <v>120</v>
       </c>
@@ -11243,7 +11386,9 @@
       <c r="D283" s="44">
         <v>12</v>
       </c>
-      <c r="E283" s="19"/>
+      <c r="E283" s="19">
+        <v>4</v>
+      </c>
       <c r="F283" s="20"/>
       <c r="G283" s="38" t="s">
         <v>64</v>
@@ -11275,12 +11420,24 @@
       <c r="P283" s="38" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="284" spans="1:27" s="11" customFormat="1" ht="15" customHeight="1">
+      <c r="AA283" s="11">
+        <v>13</v>
+      </c>
+      <c r="AB283" s="101" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="284" spans="1:28" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="F284" s="20"/>
       <c r="K284" s="45"/>
-    </row>
-    <row r="285" spans="1:27" s="47" customFormat="1" ht="23.4">
+      <c r="AA284" s="11">
+        <v>14</v>
+      </c>
+      <c r="AB284" s="101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:28" s="47" customFormat="1" ht="23.4">
       <c r="A285" s="1"/>
       <c r="B285" s="35" t="s">
         <v>43</v>
@@ -11291,7 +11448,7 @@
       <c r="D285" s="46"/>
       <c r="E285" s="19" t="str">
         <f>IF(ISERROR(E264),"",E264)&amp;";"&amp;IF(ISERROR(E265),"",E265)&amp;";"&amp;IF(ISERROR(E266),"",E266)&amp;";"&amp;IF(ISERROR(E267),"",E267)&amp;";"&amp;IF(ISERROR(E268),"",E268)&amp;";"&amp;IF(ISERROR(E269),"",E269)&amp;";"&amp;IF(ISERROR(E270),"",E270)&amp;";"&amp;IF(ISERROR(E271),"",E271)&amp;";"&amp;IF(ISERROR(E272),"",E272)&amp;";"&amp;IF(ISERROR(E273),"",E273)&amp;";"&amp;IF(ISERROR(E274),"",E274)&amp;";"&amp;IF(ISERROR(E275),"",E275)&amp;";"&amp;IF(ISERROR(E276),"",E276)&amp;";"&amp;IF(ISERROR(E277),"",E277)&amp;";"&amp;IF(ISERROR(E278),"",E278)&amp;";"&amp;IF(ISERROR(E279),"",E279)&amp;";"&amp;IF(ISERROR(E280),"",E280)&amp;";"&amp;IF(ISERROR(E281),"",E281)&amp;";"&amp;IF(ISERROR(E282),"",E282)&amp;";"&amp;IF(ISERROR(E283),"",E283)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <v>6;1;X;11;7;7;9;3;2;X;X;5;X;X;X;5;2;4;5;4</v>
       </c>
       <c r="F285" s="20"/>
       <c r="G285" s="1"/>
@@ -11314,18 +11471,35 @@
       <c r="X285" s="1"/>
       <c r="Y285" s="1"/>
       <c r="Z285" s="1"/>
-      <c r="AA285" s="1"/>
-    </row>
-    <row r="286" spans="1:27" s="11" customFormat="1" ht="15" customHeight="1">
+      <c r="AA285" s="1">
+        <v>15</v>
+      </c>
+      <c r="AB285" s="102" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="286" spans="1:28" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="F286" s="20"/>
       <c r="K286" s="45"/>
       <c r="U286" s="1"/>
-    </row>
-    <row r="287" spans="1:27" s="11" customFormat="1" ht="15" customHeight="1">
+      <c r="AA286" s="11">
+        <v>16</v>
+      </c>
+      <c r="AB286" s="101" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="287" spans="1:28" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="F287" s="20"/>
       <c r="K287" s="45"/>
-    </row>
-    <row r="288" spans="1:27">
+      <c r="AA287" s="11">
+        <v>17</v>
+      </c>
+      <c r="AB287" s="101" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="288" spans="1:28">
       <c r="B288" s="11"/>
       <c r="C288" s="11"/>
       <c r="D288" s="11"/>
@@ -11342,8 +11516,14 @@
       <c r="O288" s="11"/>
       <c r="P288" s="11"/>
       <c r="U288" s="11"/>
-    </row>
-    <row r="289" spans="2:16">
+      <c r="AA288" s="1">
+        <v>18</v>
+      </c>
+      <c r="AB288" s="103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="2:28">
       <c r="B289" s="11"/>
       <c r="C289" s="11"/>
       <c r="D289" s="11"/>
@@ -11359,9 +11539,45 @@
       <c r="N289" s="11"/>
       <c r="O289" s="11"/>
       <c r="P289" s="11"/>
+      <c r="AA289" s="1">
+        <v>19</v>
+      </c>
+      <c r="AB289" s="103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="2:28">
+      <c r="AA290" s="1">
+        <v>20</v>
+      </c>
+      <c r="AB290" s="103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="2:28">
+      <c r="AA291" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB291" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="292" spans="2:28">
+      <c r="AA292" s="1">
+        <v>22</v>
+      </c>
+      <c r="AB292" s="1">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B8:M8"/>
     <mergeCell ref="G20:M20"/>
     <mergeCell ref="G21:M21"/>
     <mergeCell ref="B23:M23"/>
@@ -11371,12 +11587,6 @@
     <mergeCell ref="G17:M17"/>
     <mergeCell ref="G18:M18"/>
     <mergeCell ref="G19:M19"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12755,8 +12965,8 @@
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:AA289"/>
   <sheetViews>
-    <sheetView topLeftCell="K255" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W268" sqref="W268"/>
+    <sheetView topLeftCell="A252" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E262" sqref="E262:E269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -12783,20 +12993,20 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1"/>
     <row r="2" spans="2:13" ht="59.25" customHeight="1">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="75"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1"/>
     <row r="4" spans="2:13" ht="33" customHeight="1">
@@ -12837,52 +13047,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
     </row>
     <row r="9" spans="2:13" ht="81" customHeight="1">
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
     </row>
     <row r="10" spans="2:13" ht="189.6" customHeight="1">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="85"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1">
       <c r="B11" s="6"/>
@@ -12962,15 +13172,15 @@
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="86" t="s">
+      <c r="G16" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="88"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="82"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="17" t="s">
@@ -12989,15 +13199,15 @@
         <f>IF(ISBLANK(Case!E17), 0, IF(E17=Case!E17, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="89" t="s">
+      <c r="G17" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="89"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="17" t="s">
@@ -13016,15 +13226,15 @@
         <f>IF(ISBLANK(Case!E18), 0, IF(E18=Case!E18, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G18" s="81" t="s">
+      <c r="G18" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="17" t="s">
@@ -13043,15 +13253,15 @@
         <f>IF(ISBLANK(Case!E19), 0, IF(E19=Case!E19, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G19" s="81" t="s">
+      <c r="G19" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="17" t="s">
@@ -13070,15 +13280,15 @@
         <f>IF(ISBLANK(Case!E20), 0, IF(E20=Case!E20, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="81" t="s">
+      <c r="G20" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="17" t="s">
@@ -13097,15 +13307,15 @@
         <f>IF(ISBLANK(Case!E21), 0, IF(E21=Case!E21, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="84"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="75"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
@@ -13162,7 +13372,7 @@
       <c r="F26" s="20"/>
       <c r="L26" s="95">
         <f>SUMPRODUCT(--(F17:F338=1),D17:D338)</f>
-        <v>760</v>
+        <v>988</v>
       </c>
       <c r="M26" s="96"/>
     </row>
@@ -18505,7 +18715,7 @@
       </c>
       <c r="F264" s="20">
         <f>IF(ISBLANK(Case!E264), 0, IF(E264=Case!E264, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G264" s="38" t="s">
         <v>145</v>
@@ -18553,7 +18763,7 @@
       </c>
       <c r="F265" s="20">
         <f>IF(ISBLANK(Case!E265), 0, IF(E265=Case!E265, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G265" s="38" t="s">
         <v>64</v>
@@ -18601,7 +18811,7 @@
       </c>
       <c r="F266" s="20">
         <f>IF(ISBLANK(Case!E266), 0, IF(E266=Case!E266, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G266" s="38" t="s">
         <v>61</v>
@@ -18649,7 +18859,7 @@
       </c>
       <c r="F267" s="20">
         <f>IF(ISBLANK(Case!E267), 0, IF(E267=Case!E267, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G267" s="38" t="s">
         <v>60</v>
@@ -18697,7 +18907,7 @@
       </c>
       <c r="F268" s="20">
         <f>IF(ISBLANK(Case!E268), 0, IF(E268=Case!E268, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G268" s="38" t="s">
         <v>145</v>
@@ -18745,7 +18955,7 @@
       </c>
       <c r="F269" s="20">
         <f>IF(ISBLANK(Case!E269), 0, IF(E269=Case!E269, 1, -1))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G269" s="38" t="s">
         <v>63</v>
@@ -18793,7 +19003,7 @@
       </c>
       <c r="F270" s="20">
         <f>IF(ISBLANK(Case!E270), 0, IF(E270=Case!E270, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G270" s="38" t="s">
         <v>145</v>
@@ -18841,7 +19051,7 @@
       </c>
       <c r="F271" s="20">
         <f>IF(ISBLANK(Case!E271), 0, IF(E271=Case!E271, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G271" s="38" t="s">
         <v>63</v>
@@ -18889,7 +19099,7 @@
       </c>
       <c r="F272" s="20">
         <f>IF(ISBLANK(Case!E272), 0, IF(E272=Case!E272, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G272" s="38" t="s">
         <v>59</v>
@@ -18937,7 +19147,7 @@
       </c>
       <c r="F273" s="20">
         <f>IF(ISBLANK(Case!E273), 0, IF(E273=Case!E273, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G273" s="38" t="s">
         <v>146</v>
@@ -18985,7 +19195,7 @@
       </c>
       <c r="F274" s="20">
         <f>IF(ISBLANK(Case!E274), 0, IF(E274=Case!E274, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G274" s="38" t="s">
         <v>58</v>
@@ -19033,7 +19243,7 @@
       </c>
       <c r="F275" s="20">
         <f>IF(ISBLANK(Case!E275), 0, IF(E275=Case!E275, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G275" s="38" t="s">
         <v>57</v>
@@ -19081,7 +19291,7 @@
       </c>
       <c r="F276" s="20">
         <f>IF(ISBLANK(Case!E276), 0, IF(E276=Case!E276, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G276" s="38" t="s">
         <v>60</v>
@@ -19129,7 +19339,7 @@
       </c>
       <c r="F277" s="20">
         <f>IF(ISBLANK(Case!E277), 0, IF(E277=Case!E277, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G277" s="38" t="s">
         <v>57</v>
@@ -19177,7 +19387,7 @@
       </c>
       <c r="F278" s="20">
         <f>IF(ISBLANK(Case!E278), 0, IF(E278=Case!E278, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G278" s="38" t="s">
         <v>146</v>
@@ -19225,7 +19435,7 @@
       </c>
       <c r="F279" s="20">
         <f>IF(ISBLANK(Case!E279), 0, IF(E279=Case!E279, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G279" s="38" t="s">
         <v>62</v>
@@ -19273,7 +19483,7 @@
       </c>
       <c r="F280" s="20">
         <f>IF(ISBLANK(Case!E280), 0, IF(E280=Case!E280, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G280" s="38" t="s">
         <v>59</v>
@@ -19321,7 +19531,7 @@
       </c>
       <c r="F281" s="20">
         <f>IF(ISBLANK(Case!E281), 0, IF(E281=Case!E281, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G281" s="38" t="s">
         <v>147</v>
@@ -19369,7 +19579,7 @@
       </c>
       <c r="F282" s="20">
         <f>IF(ISBLANK(Case!E282), 0, IF(E282=Case!E282, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G282" s="38" t="s">
         <v>64</v>
@@ -19417,7 +19627,7 @@
       </c>
       <c r="F283" s="20">
         <f>IF(ISBLANK(Case!E283), 0, IF(E283=Case!E283, 1, -1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G283" s="38" t="s">
         <v>64</v>
@@ -19534,11 +19744,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G20:M20"/>
-    <mergeCell ref="G21:M21"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M28"/>
     <mergeCell ref="G19:M19"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B4:J4"/>
@@ -19551,6 +19756,11 @@
     <mergeCell ref="G16:M16"/>
     <mergeCell ref="G17:M17"/>
     <mergeCell ref="G18:M18"/>
+    <mergeCell ref="G20:M20"/>
+    <mergeCell ref="G21:M21"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Good progress- nearly done
</commit_message>
<xml_diff>
--- a/2025 Excel Esports Chille - The Docks of Valparaiso (Juan Jose Cifuentes) - Case and Answers.xlsx
+++ b/2025 Excel Esports Chille - The Docks of Valparaiso (Juan Jose Cifuentes) - Case and Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0506AA6-BA04-4A29-B758-A10108D144E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1006E5-E9A2-4678-8189-D733DE778769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE4A18CD-9E80-4D14-A39F-1C9BD96D766A}"/>
   </bookViews>
@@ -1524,6 +1524,15 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1610,15 +1619,6 @@
     </xf>
     <xf numFmtId="3" fontId="27" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2948,10 +2948,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E46771-3E32-4515-837B-D61C1E8E2229}">
   <sheetPr codeName="Sheet28"/>
-  <dimension ref="A1:AE292"/>
+  <dimension ref="A1:AG292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S260" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z268" sqref="Z268:Z271"/>
+    <sheetView tabSelected="1" topLeftCell="W254" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF261" sqref="AF261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.8984375" defaultRowHeight="14.4"/>
@@ -2974,39 +2974,39 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1"/>
     <row r="2" spans="2:13" ht="59.25" customHeight="1">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="90"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1"/>
     <row r="4" spans="2:13" ht="33" customHeight="1">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="78"/>
+      <c r="M4" s="81"/>
     </row>
     <row r="5" spans="2:13" ht="196.2" customHeight="1">
       <c r="C5"/>
@@ -3017,10 +3017,10 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:13" ht="33" customHeight="1">
-      <c r="L6" s="76" t="s">
+      <c r="L6" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="78"/>
+      <c r="M6" s="81"/>
     </row>
     <row r="7" spans="2:13" ht="113.4" customHeight="1">
       <c r="K7" s="4"/>
@@ -3028,52 +3028,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
     </row>
     <row r="9" spans="2:13" ht="79.2" customHeight="1">
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
     </row>
     <row r="10" spans="2:13" ht="194.4" customHeight="1">
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1">
       <c r="B11" s="5"/>
@@ -3090,20 +3090,20 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="78"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="81"/>
     </row>
     <row r="13" spans="2:13" ht="15" customHeight="1">
       <c r="B13" s="8"/>
@@ -3153,15 +3153,15 @@
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="80" t="s">
+      <c r="G16" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="82"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="85"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="16" t="s">
@@ -3175,15 +3175,15 @@
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="83" t="s">
+      <c r="G17" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="16" t="s">
@@ -3197,15 +3197,15 @@
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="72" t="s">
+      <c r="G18" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="16" t="s">
@@ -3219,15 +3219,15 @@
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="72" t="s">
+      <c r="G19" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="16" t="s">
@@ -3241,15 +3241,15 @@
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="16" t="s">
@@ -3263,34 +3263,34 @@
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="73" t="s">
+      <c r="G21" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="75"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.4">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="78"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="81"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="24"/>
@@ -10005,7 +10005,7 @@
       <c r="F256" s="20"/>
       <c r="G256" s="28"/>
     </row>
-    <row r="257" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="257" spans="2:33" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B257" s="32" t="s">
         <v>160</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="258" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="258" spans="2:33" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B258" s="32" t="s">
         <v>161</v>
       </c>
@@ -10028,7 +10028,7 @@
       <c r="F258" s="20"/>
       <c r="G258" s="28"/>
     </row>
-    <row r="259" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="259" spans="2:33" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="B259" s="29"/>
       <c r="C259" s="20"/>
       <c r="D259" s="20"/>
@@ -10036,7 +10036,7 @@
       <c r="F259" s="20"/>
       <c r="G259" s="28"/>
     </row>
-    <row r="260" spans="2:31" s="11" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
+    <row r="260" spans="2:33" s="11" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
       <c r="B260" s="13" t="s">
         <v>10</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="261" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="261" spans="2:33" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="F261" s="20"/>
       <c r="U261" s="67" t="s">
         <v>53</v>
@@ -10141,8 +10141,16 @@
         <f t="array" aca="1" ref="AE261:AE262" ca="1">_xlfn.SCAN(0,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(AB261),3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v))</f>
         <v>115600.00000000001</v>
       </c>
-    </row>
-    <row r="262" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
+      <c r="AF261" s="11" t="str" cm="1">
+        <f t="array" aca="1" ref="AF261" ca="1">INDEX(X268:X271,_xlfn.XMATCH(AD261,_xlfn.ANCHORARRAY(Z268),1))</f>
+        <v>DBL4</v>
+      </c>
+      <c r="AG261" s="11">
+        <f ca="1">_xlfn.XMATCH(AF261,_xlfn.TAKE(_xlfn.ANCHORARRAY(X268),,1))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
       <c r="B262" s="35" t="s">
         <v>164</v>
       </c>
@@ -10219,7 +10227,7 @@
         <v>207400</v>
       </c>
     </row>
-    <row r="263" spans="2:31" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="263" spans="2:33" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="E263" s="40"/>
       <c r="F263" s="20"/>
       <c r="G263" s="41"/>
@@ -10249,7 +10257,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="264" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="264" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B264" s="43">
         <v>101</v>
       </c>
@@ -10310,7 +10318,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="265" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="265" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B265" s="43">
         <v>102</v>
       </c>
@@ -10383,7 +10391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="266" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="266" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B266" s="43">
         <v>103</v>
       </c>
@@ -10428,7 +10436,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="267" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="267" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
       <c r="B267" s="43">
         <v>104</v>
       </c>
@@ -10486,7 +10494,7 @@
       </c>
       <c r="Z267"/>
     </row>
-    <row r="268" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
+    <row r="268" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1" thickTop="1">
       <c r="B268" s="43">
         <v>105</v>
       </c>
@@ -10554,7 +10562,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="269" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="269" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B269" s="43">
         <v>106</v>
       </c>
@@ -10617,7 +10625,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="270" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="270" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B270" s="43">
         <v>107</v>
       </c>
@@ -10680,7 +10688,7 @@
         <v>335000</v>
       </c>
     </row>
-    <row r="271" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="271" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B271" s="43">
         <v>108</v>
       </c>
@@ -10743,7 +10751,7 @@
         <v>395000</v>
       </c>
     </row>
-    <row r="272" spans="2:31" s="11" customFormat="1" ht="23.25" customHeight="1">
+    <row r="272" spans="2:33" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="B272" s="43">
         <v>109</v>
       </c>
@@ -10858,7 +10866,7 @@
         <f t="array" ref="AA273:AA292">_xlfn.SEQUENCE(20,1,3)</f>
         <v>3</v>
       </c>
-      <c r="AB273" s="101">
+      <c r="AB273" s="72">
         <f t="dataTable" ref="AB273:AB292" dt2D="0" dtr="0" r1="V260" ca="1"/>
         <v>6</v>
       </c>
@@ -10919,7 +10927,7 @@
       <c r="AA274" s="11">
         <v>4</v>
       </c>
-      <c r="AB274" s="101">
+      <c r="AB274" s="72">
         <v>1</v>
       </c>
     </row>
@@ -10979,7 +10987,7 @@
       <c r="AA275" s="11">
         <v>5</v>
       </c>
-      <c r="AB275" s="101" t="str">
+      <c r="AB275" s="72" t="str">
         <v>X</v>
       </c>
     </row>
@@ -11039,7 +11047,7 @@
       <c r="AA276" s="11">
         <v>6</v>
       </c>
-      <c r="AB276" s="101">
+      <c r="AB276" s="72">
         <v>11</v>
       </c>
     </row>
@@ -11099,7 +11107,7 @@
       <c r="AA277" s="11">
         <v>7</v>
       </c>
-      <c r="AB277" s="101">
+      <c r="AB277" s="72">
         <v>7</v>
       </c>
     </row>
@@ -11159,7 +11167,7 @@
       <c r="AA278" s="11">
         <v>8</v>
       </c>
-      <c r="AB278" s="101">
+      <c r="AB278" s="72">
         <v>7</v>
       </c>
     </row>
@@ -11219,7 +11227,7 @@
       <c r="AA279" s="11">
         <v>9</v>
       </c>
-      <c r="AB279" s="101">
+      <c r="AB279" s="72">
         <v>9</v>
       </c>
     </row>
@@ -11270,7 +11278,7 @@
       <c r="AA280" s="11">
         <v>10</v>
       </c>
-      <c r="AB280" s="101">
+      <c r="AB280" s="72">
         <v>3</v>
       </c>
     </row>
@@ -11321,7 +11329,7 @@
       <c r="AA281" s="11">
         <v>11</v>
       </c>
-      <c r="AB281" s="101">
+      <c r="AB281" s="72">
         <v>2</v>
       </c>
     </row>
@@ -11372,7 +11380,7 @@
       <c r="AA282" s="11">
         <v>12</v>
       </c>
-      <c r="AB282" s="101" t="str">
+      <c r="AB282" s="72" t="str">
         <v>X</v>
       </c>
     </row>
@@ -11423,7 +11431,7 @@
       <c r="AA283" s="11">
         <v>13</v>
       </c>
-      <c r="AB283" s="101" t="str">
+      <c r="AB283" s="72" t="str">
         <v>X</v>
       </c>
     </row>
@@ -11433,7 +11441,7 @@
       <c r="AA284" s="11">
         <v>14</v>
       </c>
-      <c r="AB284" s="101">
+      <c r="AB284" s="72">
         <v>5</v>
       </c>
     </row>
@@ -11474,7 +11482,7 @@
       <c r="AA285" s="1">
         <v>15</v>
       </c>
-      <c r="AB285" s="102" t="str">
+      <c r="AB285" s="73" t="str">
         <v>X</v>
       </c>
     </row>
@@ -11485,7 +11493,7 @@
       <c r="AA286" s="11">
         <v>16</v>
       </c>
-      <c r="AB286" s="101" t="str">
+      <c r="AB286" s="72" t="str">
         <v>X</v>
       </c>
     </row>
@@ -11495,7 +11503,7 @@
       <c r="AA287" s="11">
         <v>17</v>
       </c>
-      <c r="AB287" s="101" t="str">
+      <c r="AB287" s="72" t="str">
         <v>X</v>
       </c>
     </row>
@@ -11519,7 +11527,7 @@
       <c r="AA288" s="1">
         <v>18</v>
       </c>
-      <c r="AB288" s="103">
+      <c r="AB288" s="74">
         <v>5</v>
       </c>
     </row>
@@ -11542,7 +11550,7 @@
       <c r="AA289" s="1">
         <v>19</v>
       </c>
-      <c r="AB289" s="103">
+      <c r="AB289" s="74">
         <v>2</v>
       </c>
     </row>
@@ -11550,7 +11558,7 @@
       <c r="AA290" s="1">
         <v>20</v>
       </c>
-      <c r="AB290" s="103">
+      <c r="AB290" s="74">
         <v>4</v>
       </c>
     </row>
@@ -11905,15 +11913,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.95" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="95"/>
     </row>
     <row r="2" spans="1:7" ht="16.95" customHeight="1">
       <c r="A2" s="60" t="s">
@@ -12518,11 +12526,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.95" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="93" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
     </row>
     <row r="2" spans="1:3" ht="16.8" customHeight="1">
       <c r="A2" s="60" t="s">
@@ -12766,19 +12774,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.95" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="93" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="95"/>
     </row>
     <row r="2" spans="1:4" ht="16.95" customHeight="1">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="96" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="94"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
     </row>
     <row r="3" spans="1:4" ht="16.95" customHeight="1">
       <c r="A3" s="63" t="s">
@@ -12993,39 +13001,39 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1"/>
     <row r="2" spans="2:13" ht="59.25" customHeight="1">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="90"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1"/>
     <row r="4" spans="2:13" ht="33" customHeight="1">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="78"/>
+      <c r="M4" s="81"/>
     </row>
     <row r="5" spans="2:13" ht="196.2" customHeight="1">
       <c r="C5"/>
@@ -13036,10 +13044,10 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:13" ht="33" customHeight="1">
-      <c r="L6" s="76" t="s">
+      <c r="L6" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="78"/>
+      <c r="M6" s="81"/>
     </row>
     <row r="7" spans="2:13" ht="113.4" customHeight="1">
       <c r="K7" s="4"/>
@@ -13047,52 +13055,52 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
     </row>
     <row r="9" spans="2:13" ht="81" customHeight="1">
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
     </row>
     <row r="10" spans="2:13" ht="189.6" customHeight="1">
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
     </row>
     <row r="11" spans="2:13" ht="15" customHeight="1">
       <c r="B11" s="6"/>
@@ -13109,20 +13117,20 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" ht="21.75" customHeight="1">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="78"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="81"/>
     </row>
     <row r="13" spans="2:13" ht="15" customHeight="1">
       <c r="B13" s="8"/>
@@ -13172,15 +13180,15 @@
         <v>13</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="80" t="s">
+      <c r="G16" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="82"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="85"/>
     </row>
     <row r="17" spans="2:13" ht="37.5" customHeight="1">
       <c r="B17" s="17" t="s">
@@ -13199,15 +13207,15 @@
         <f>IF(ISBLANK(Case!E17), 0, IF(E17=Case!E17, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="83" t="s">
+      <c r="G17" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1">
       <c r="B18" s="17" t="s">
@@ -13226,15 +13234,15 @@
         <f>IF(ISBLANK(Case!E18), 0, IF(E18=Case!E18, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G18" s="72" t="s">
+      <c r="G18" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
     </row>
     <row r="19" spans="2:13" ht="37.5" customHeight="1">
       <c r="B19" s="17" t="s">
@@ -13253,15 +13261,15 @@
         <f>IF(ISBLANK(Case!E19), 0, IF(E19=Case!E19, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G19" s="72" t="s">
+      <c r="G19" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
     </row>
     <row r="20" spans="2:13" ht="37.5" customHeight="1">
       <c r="B20" s="17" t="s">
@@ -13280,15 +13288,15 @@
         <f>IF(ISBLANK(Case!E20), 0, IF(E20=Case!E20, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="G20" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
     </row>
     <row r="21" spans="2:13" ht="37.5" customHeight="1">
       <c r="B21" s="17" t="s">
@@ -13307,34 +13315,34 @@
         <f>IF(ISBLANK(Case!E21), 0, IF(E21=Case!E21, 1, -1))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G21" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="75"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1">
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:13" ht="23.4">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="78"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="81"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="24"/>
@@ -13360,21 +13368,21 @@
       <c r="D25" s="20"/>
       <c r="E25" s="28"/>
       <c r="F25" s="20"/>
-      <c r="L25" s="76" t="s">
+      <c r="L25" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="M25" s="78"/>
+      <c r="M25" s="81"/>
     </row>
     <row r="26" spans="2:13" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="B26" s="29"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
-      <c r="L26" s="95">
+      <c r="L26" s="98">
         <f>SUMPRODUCT(--(F17:F338=1),D17:D338)</f>
         <v>988</v>
       </c>
-      <c r="M26" s="96"/>
+      <c r="M26" s="99"/>
     </row>
     <row r="27" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B27" s="28" t="s">
@@ -13384,8 +13392,8 @@
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="L27" s="97"/>
-      <c r="M27" s="98"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="101"/>
     </row>
     <row r="28" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B28" s="30"/>
@@ -13393,8 +13401,8 @@
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="L28" s="99"/>
-      <c r="M28" s="100"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="103"/>
     </row>
     <row r="29" spans="2:13" s="11" customFormat="1" ht="14.4" customHeight="1">
       <c r="B29" s="31" t="s">

</xml_diff>